<commit_message>
more work on adding time to caps; more data cleaning
</commit_message>
<xml_diff>
--- a/data/botw_otherdata2.xlsx
+++ b/data/botw_otherdata2.xlsx
@@ -9793,6 +9793,11 @@
           <t>N/A (spotlight)</t>
         </is>
       </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>00:00 - 29:43</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172">
@@ -10188,6 +10193,11 @@
           <t>N/A (spotlight)</t>
         </is>
       </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>00:00 - 38:52</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179">
@@ -10566,6 +10576,11 @@
       <c r="I185" t="inlineStr">
         <is>
           <t>N/A (spotlight)</t>
+        </is>
+      </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>00:00 - 39:20</t>
         </is>
       </c>
     </row>

</xml_diff>